<commit_message>
BOMs update (mouser and PCB)
</commit_message>
<xml_diff>
--- a/- PCB -/SUMEC SMD/BOM/sumec PCB BOM.xlsx
+++ b/- PCB -/SUMEC SMD/BOM/sumec PCB BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\Рабочий стол\GitHub\RoboCop\- PCB -\SUMEC SMD\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D6527F5-7E11-41D7-BB62-A1CC9F266E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CAB930-4B0C-4039-A44E-218DF8300259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sumec" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="132">
   <si>
     <t>Item</t>
   </si>
@@ -370,12 +370,6 @@
     <t>10uF 16V mouser</t>
   </si>
   <si>
-    <t>1uf 16V mouser</t>
-  </si>
-  <si>
-    <t>0,1uF 16V mouser</t>
-  </si>
-  <si>
     <t>USB C mouser</t>
   </si>
   <si>
@@ -410,12 +404,24 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Tantal. 10uF, 25V mouser</t>
+  </si>
+  <si>
+    <t>Tantal, 1uf 16V mouser</t>
+  </si>
+  <si>
+    <t>0,1uF 25V</t>
+  </si>
+  <si>
+    <t>Schottkyho dioda 1206 2A propustny proud</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -566,7 +572,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -791,6 +797,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1008,26 +1020,27 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="41" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % – Zvýraznění 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1383,11 +1396,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="92" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1406,25 +1419,25 @@
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="10" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1438,7 +1451,7 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1447,8 +1460,8 @@
       <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>115</v>
+      <c r="G6" s="14" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -1461,7 +1474,7 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1470,8 +1483,8 @@
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>116</v>
+      <c r="G7" s="14" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -1493,7 +1506,7 @@
       <c r="F8" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1516,8 +1529,8 @@
       <c r="F9" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>117</v>
+      <c r="G9" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -1539,7 +1552,7 @@
       <c r="F10" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1562,8 +1575,8 @@
       <c r="F11" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>117</v>
+      <c r="G11" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -1585,8 +1598,8 @@
       <c r="F12" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>117</v>
+      <c r="G12" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -1608,8 +1621,8 @@
       <c r="F13" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>117</v>
+      <c r="G13" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -1631,8 +1644,8 @@
       <c r="F14" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>117</v>
+      <c r="G14" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -1651,10 +1664,10 @@
       <c r="E15" t="s">
         <v>96</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1674,10 +1687,12 @@
       <c r="E16" t="s">
         <v>103</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="1"/>
+      <c r="G16" s="14" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
@@ -1698,7 +1713,7 @@
       <c r="F17" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="13"/>
+      <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
@@ -1719,7 +1734,7 @@
       <c r="F18" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="13"/>
+      <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
@@ -1740,7 +1755,7 @@
       <c r="F19" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="13"/>
+      <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
@@ -1761,7 +1776,7 @@
       <c r="F20" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="13"/>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
@@ -1782,7 +1797,7 @@
       <c r="F21" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="13"/>
+      <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
@@ -1803,8 +1818,8 @@
       <c r="F22" t="s">
         <v>47</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>118</v>
+      <c r="G22" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1826,8 +1841,8 @@
       <c r="F23" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>119</v>
+      <c r="G23" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -1849,7 +1864,7 @@
       <c r="F24" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="13"/>
+      <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
@@ -1870,7 +1885,7 @@
       <c r="F25" t="s">
         <v>57</v>
       </c>
-      <c r="G25" s="13"/>
+      <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
@@ -1891,7 +1906,7 @@
       <c r="F26" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="13"/>
+      <c r="G26" s="11"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
@@ -1912,7 +1927,7 @@
       <c r="F27" t="s">
         <v>62</v>
       </c>
-      <c r="G27" s="13"/>
+      <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
@@ -1933,8 +1948,8 @@
       <c r="F28" t="s">
         <v>65</v>
       </c>
-      <c r="G28" s="4" t="s">
-        <v>123</v>
+      <c r="G28" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1956,8 +1971,8 @@
       <c r="F29" t="s">
         <v>65</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>129</v>
+      <c r="G29" s="15" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -1979,8 +1994,8 @@
       <c r="F30" t="s">
         <v>65</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>129</v>
+      <c r="G30" s="15" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -1993,7 +2008,7 @@
       <c r="C31" t="s">
         <v>70</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>95</v>
       </c>
       <c r="E31" t="s">
@@ -2002,8 +2017,8 @@
       <c r="F31" t="s">
         <v>65</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>129</v>
+      <c r="G31" s="15" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -2025,8 +2040,8 @@
       <c r="F32" t="s">
         <v>65</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>129</v>
+      <c r="G32" s="15" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -2048,8 +2063,8 @@
       <c r="F33" t="s">
         <v>75</v>
       </c>
-      <c r="G33" s="4" t="s">
-        <v>128</v>
+      <c r="G33" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -2071,8 +2086,8 @@
       <c r="F34" t="s">
         <v>78</v>
       </c>
-      <c r="G34" s="4" t="s">
-        <v>124</v>
+      <c r="G34" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -2094,8 +2109,8 @@
       <c r="F35" t="s">
         <v>81</v>
       </c>
-      <c r="G35" s="4" t="s">
-        <v>122</v>
+      <c r="G35" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -2117,8 +2132,8 @@
       <c r="F36" t="s">
         <v>84</v>
       </c>
-      <c r="G36" s="4" t="s">
-        <v>121</v>
+      <c r="G36" s="3" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -2140,8 +2155,8 @@
       <c r="F37" t="s">
         <v>45</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>125</v>
+      <c r="G37" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -2163,8 +2178,8 @@
       <c r="F38" t="s">
         <v>89</v>
       </c>
-      <c r="G38" s="4" t="s">
-        <v>120</v>
+      <c r="G38" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -2186,8 +2201,8 @@
       <c r="F39" t="s">
         <v>92</v>
       </c>
-      <c r="G39" s="4" t="s">
-        <v>126</v>
+      <c r="G39" s="14" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -2209,31 +2224,32 @@
       <c r="F40" t="s">
         <v>92</v>
       </c>
-      <c r="G40" s="4" t="s">
-        <v>127</v>
+      <c r="G40" s="14" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G8" r:id="rId1" display="10uF 16V"/>
-    <hyperlink ref="G10" r:id="rId2" display="10uF 16V"/>
-    <hyperlink ref="G15" r:id="rId3" display="10uF 16V"/>
-    <hyperlink ref="G11" r:id="rId4" display="0,1uF 16V"/>
-    <hyperlink ref="G9" r:id="rId5" display="0,1uF 16V"/>
-    <hyperlink ref="G6" r:id="rId6" display="10uF 16V"/>
-    <hyperlink ref="G7" r:id="rId7" display="1uf 16V"/>
-    <hyperlink ref="G22" r:id="rId8" display="USB C"/>
-    <hyperlink ref="G12:G14" r:id="rId9" display="0,1uF 16V"/>
-    <hyperlink ref="G23" r:id="rId10" display="JST SH 6 pin 1mm"/>
-    <hyperlink ref="G28" r:id="rId11" display="0R"/>
-    <hyperlink ref="G35" r:id="rId12" display="ESP32 S3 WROOM1"/>
-    <hyperlink ref="G36" r:id="rId13" display="ESD protekce"/>
-    <hyperlink ref="G38" r:id="rId14" display="QRE1113 THT"/>
-    <hyperlink ref="G39" r:id="rId15" display="TO-252-3, 1,5A 5V"/>
-    <hyperlink ref="G40" r:id="rId16" display="TO-252-3, 1,5A, 3.3Vout"/>
-    <hyperlink ref="G37" r:id="rId17" display="TSOP382. 38kHz"/>
-    <hyperlink ref="G34" r:id="rId18"/>
-    <hyperlink ref="G33" r:id="rId19"/>
+    <hyperlink ref="G8" r:id="rId1" display="10uF 16V" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G10" r:id="rId2" display="10uF 16V" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G15" r:id="rId3" display="10uF 16V" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G22" r:id="rId5" display="USB C" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G23" r:id="rId6" display="JST SH 6 pin 1mm" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G28" r:id="rId7" display="0R" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G35" r:id="rId8" display="ESP32 S3 WROOM1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G36" r:id="rId9" display="ESD protekce" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G38" r:id="rId10" display="QRE1113 THT" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G39" r:id="rId11" display="TO-252-3, 1,5A 5V" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G40" r:id="rId12" display="TO-252-3, 1,5A, 3.3Vout" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G37" r:id="rId13" display="TSOP382. 38kHz" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G34" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G33" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G6" r:id="rId16" display="Tantal. 10uF, 25V" xr:uid="{B359CBE2-F8FE-4E17-BFBE-5ECF82A020EF}"/>
+    <hyperlink ref="G9" r:id="rId17" display="0,1uF 16V" xr:uid="{41803D5A-EA45-4A1E-AA2E-5BF158BCA741}"/>
+    <hyperlink ref="G11" r:id="rId18" display="0,1uF 16V" xr:uid="{76EDC6BD-6363-4848-8D03-214E1E821E90}"/>
+    <hyperlink ref="G12:G14" r:id="rId19" display="0,1uF 16V" xr:uid="{F49C0BF7-169A-4EDA-8738-A7D0665B10B4}"/>
+    <hyperlink ref="G16" r:id="rId20" xr:uid="{A3B90A94-2E04-49DA-BD43-0A4BBCBA18A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Brom bom bom bom update
</commit_message>
<xml_diff>
--- a/- PCB -/SUMEC SMD/BOM/sumec PCB BOM.xlsx
+++ b/- PCB -/SUMEC SMD/BOM/sumec PCB BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\Рабочий стол\GitHub\RoboCop\- PCB -\SUMEC SMD\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD1EDA5-D4EE-40B6-9DD0-5AAFC78A06C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F60156-45CA-4786-882C-BF200BDBF07A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1026,7 +1026,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1047,6 +1047,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" xfId="42" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % – Zvýraznění 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1405,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="92" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="82" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2115,7 +2116,7 @@
       <c r="F35" t="s">
         <v>81</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="16" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2161,7 +2162,7 @@
       <c r="F37" t="s">
         <v>45</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="16" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2248,18 +2249,18 @@
     <hyperlink ref="G38" r:id="rId10" display="QRE1113 THT" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="G39" r:id="rId11" display="TO-252-3, 1,5A 5V" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="G40" r:id="rId12" display="TO-252-3, 1,5A, 3.3Vout" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G37" r:id="rId13" display="TSOP382. 38kHz" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G34" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G33" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G6" r:id="rId16" display="Tantal. 10uF, 25V" xr:uid="{B359CBE2-F8FE-4E17-BFBE-5ECF82A020EF}"/>
-    <hyperlink ref="G9" r:id="rId17" display="0,1uF 16V" xr:uid="{41803D5A-EA45-4A1E-AA2E-5BF158BCA741}"/>
-    <hyperlink ref="G11" r:id="rId18" display="0,1uF 16V" xr:uid="{76EDC6BD-6363-4848-8D03-214E1E821E90}"/>
-    <hyperlink ref="G12:G14" r:id="rId19" display="0,1uF 16V" xr:uid="{F49C0BF7-169A-4EDA-8738-A7D0665B10B4}"/>
-    <hyperlink ref="G16" r:id="rId20" xr:uid="{A3B90A94-2E04-49DA-BD43-0A4BBCBA18A0}"/>
-    <hyperlink ref="G30" r:id="rId21" xr:uid="{AA9044A8-CE50-4E37-AA82-8E5E514EF54B}"/>
-    <hyperlink ref="G32" r:id="rId22" xr:uid="{A5BB3475-2E73-4B3C-9D26-2667A0D1CCD2}"/>
-    <hyperlink ref="G31" r:id="rId23" xr:uid="{B0E11761-34DD-4E90-ABC6-BF91DEF1FAAA}"/>
-    <hyperlink ref="G29" r:id="rId24" xr:uid="{FE390BCC-300F-469D-93F8-35DBC09A86FE}"/>
+    <hyperlink ref="G34" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G33" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G6" r:id="rId15" display="Tantal. 10uF, 25V" xr:uid="{B359CBE2-F8FE-4E17-BFBE-5ECF82A020EF}"/>
+    <hyperlink ref="G9" r:id="rId16" display="0,1uF 16V" xr:uid="{41803D5A-EA45-4A1E-AA2E-5BF158BCA741}"/>
+    <hyperlink ref="G11" r:id="rId17" display="0,1uF 16V" xr:uid="{76EDC6BD-6363-4848-8D03-214E1E821E90}"/>
+    <hyperlink ref="G12:G14" r:id="rId18" display="0,1uF 16V" xr:uid="{F49C0BF7-169A-4EDA-8738-A7D0665B10B4}"/>
+    <hyperlink ref="G16" r:id="rId19" xr:uid="{A3B90A94-2E04-49DA-BD43-0A4BBCBA18A0}"/>
+    <hyperlink ref="G30" r:id="rId20" xr:uid="{AA9044A8-CE50-4E37-AA82-8E5E514EF54B}"/>
+    <hyperlink ref="G32" r:id="rId21" xr:uid="{A5BB3475-2E73-4B3C-9D26-2667A0D1CCD2}"/>
+    <hyperlink ref="G31" r:id="rId22" xr:uid="{B0E11761-34DD-4E90-ABC6-BF91DEF1FAAA}"/>
+    <hyperlink ref="G29" r:id="rId23" xr:uid="{FE390BCC-300F-469D-93F8-35DBC09A86FE}"/>
+    <hyperlink ref="G37" r:id="rId24" display="TSOP382. 38kHz" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sumec SMD V2 schematic update
</commit_message>
<xml_diff>
--- a/- PCB -/SUMEC SMD/BOM/sumec PCB BOM.xlsx
+++ b/- PCB -/SUMEC SMD/BOM/sumec PCB BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\Рабочий стол\GitHub\RoboCop\- PCB -\SUMEC SMD\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\RoboCop\- PCB -\SUMEC SMD\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F60156-45CA-4786-882C-BF200BDBF07A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F407EEE-947E-45C1-B33D-A6D9F0B344B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sumec" sheetId="1" r:id="rId1"/>
@@ -1080,8 +1080,8 @@
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
     <cellStyle name="Poznámka" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Propojená buňka" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Správně" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Špatně" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Správně" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Text upozornění" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Vstup" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Výpočet" xfId="11" builtinId="22" customBuiltin="1"/>
@@ -1406,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="82" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="D9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>